<commit_message>
Benutzer und Kinder auflisten
</commit_message>
<xml_diff>
--- a/Taetigkeitsprotokolle/Taetigkeitsprotokoll_Kollross.xlsx
+++ b/Taetigkeitsprotokolle/Taetigkeitsprotokoll_Kollross.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Datum</t>
   </si>
@@ -88,6 +88,12 @@
   </si>
   <si>
     <t>Sprintplanung</t>
+  </si>
+  <si>
+    <t>26.11.2019</t>
+  </si>
+  <si>
+    <t>Benutzer und Kinder auflisten</t>
   </si>
 </sst>
 </file>
@@ -285,6 +291,18 @@
     <xf numFmtId="166" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -308,18 +326,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -358,7 +364,7 @@
         <xdr:cNvPr id="2" name="Grafik 1" descr="H:\HTL-Logodaten\HTL_Raster_Farbe_auf_transparent_komplett_Größe_1.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -686,7 +692,7 @@
   <dimension ref="A1:M50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -699,12 +705,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="4" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
       <c r="G1" s="8"/>
@@ -741,35 +747,35 @@
       <c r="G4" s="10"/>
     </row>
     <row r="5" spans="1:13" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="31" t="s">
+      <c r="B5" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="31"/>
-      <c r="E5" s="35" t="s">
+      <c r="D5" s="35"/>
+      <c r="E5" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="35" t="s">
+      <c r="F5" s="39" t="s">
         <v>5</v>
       </c>
       <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:13" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="36"/>
-      <c r="B6" s="36"/>
+      <c r="A6" s="40"/>
+      <c r="B6" s="40"/>
       <c r="C6" s="21" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
       <c r="G6" s="8"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
@@ -821,12 +827,12 @@
         <v>5.555555555555558E-2</v>
       </c>
       <c r="G8" s="11"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="32"/>
-      <c r="L8" s="32"/>
-      <c r="M8" s="32"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="36"/>
     </row>
     <row r="9" spans="1:13" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
@@ -852,14 +858,24 @@
       <c r="J9" s="3"/>
     </row>
     <row r="10" spans="1:13" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="23"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="27"/>
+      <c r="A10" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="25">
+        <v>0.32291666666666669</v>
+      </c>
+      <c r="D10" s="25">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>22</v>
+      </c>
       <c r="F10" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.19791666666666669</v>
       </c>
       <c r="G10" s="11"/>
       <c r="J10" s="3"/>
@@ -1191,109 +1207,109 @@
       <c r="G37" s="11"/>
     </row>
     <row r="38" spans="1:7" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="29" t="s">
+      <c r="A38" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="29"/>
-      <c r="C38" s="29"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="29"/>
+      <c r="B38" s="33"/>
+      <c r="C38" s="33"/>
+      <c r="D38" s="33"/>
+      <c r="E38" s="33"/>
       <c r="F38" s="22">
         <f>SUM(F7:F37)</f>
-        <v>0.35069444444444448</v>
+        <v>0.54861111111111116</v>
       </c>
       <c r="G38" s="8"/>
     </row>
     <row r="39" spans="1:7" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="38"/>
-      <c r="B39" s="38"/>
-      <c r="C39" s="38"/>
-      <c r="D39" s="38"/>
-      <c r="E39" s="38"/>
-      <c r="F39" s="38"/>
+      <c r="A39" s="30"/>
+      <c r="B39" s="30"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="30"/>
       <c r="G39" s="8"/>
     </row>
     <row r="40" spans="1:7" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="30" t="s">
+      <c r="A40" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B40" s="30"/>
-      <c r="C40" s="30"/>
-      <c r="D40" s="30"/>
-      <c r="E40" s="30"/>
-      <c r="F40" s="30"/>
+      <c r="B40" s="34"/>
+      <c r="C40" s="34"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="34"/>
       <c r="G40" s="8"/>
     </row>
     <row r="41" spans="1:7" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A41" s="39"/>
-      <c r="B41" s="39"/>
-      <c r="C41" s="39"/>
-      <c r="D41" s="39"/>
-      <c r="E41" s="39"/>
-      <c r="F41" s="39"/>
+      <c r="A41" s="31"/>
+      <c r="B41" s="31"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="31"/>
       <c r="G41" s="8"/>
     </row>
     <row r="42" spans="1:7" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="40"/>
-      <c r="B42" s="40"/>
-      <c r="C42" s="40"/>
-      <c r="D42" s="40"/>
-      <c r="E42" s="40"/>
-      <c r="F42" s="40"/>
+      <c r="A42" s="32"/>
+      <c r="B42" s="32"/>
+      <c r="C42" s="32"/>
+      <c r="D42" s="32"/>
+      <c r="E42" s="32"/>
+      <c r="F42" s="32"/>
       <c r="G42" s="8"/>
     </row>
     <row r="43" spans="1:7" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="37"/>
-      <c r="B43" s="37"/>
-      <c r="C43" s="37"/>
-      <c r="D43" s="37"/>
-      <c r="E43" s="37"/>
-      <c r="F43" s="37"/>
+      <c r="A43" s="29"/>
+      <c r="B43" s="29"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="29"/>
+      <c r="F43" s="29"/>
       <c r="G43" s="8"/>
     </row>
     <row r="44" spans="1:7" s="4" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="37"/>
-      <c r="B44" s="37"/>
-      <c r="C44" s="37"/>
-      <c r="D44" s="37"/>
-      <c r="E44" s="37"/>
-      <c r="F44" s="37"/>
+      <c r="A44" s="29"/>
+      <c r="B44" s="29"/>
+      <c r="C44" s="29"/>
+      <c r="D44" s="29"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="29"/>
       <c r="G44" s="8"/>
     </row>
     <row r="45" spans="1:7" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A45" s="37"/>
-      <c r="B45" s="37"/>
-      <c r="C45" s="37"/>
-      <c r="D45" s="37"/>
-      <c r="E45" s="37"/>
-      <c r="F45" s="37"/>
+      <c r="A45" s="29"/>
+      <c r="B45" s="29"/>
+      <c r="C45" s="29"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="29"/>
+      <c r="F45" s="29"/>
       <c r="G45" s="8"/>
     </row>
     <row r="46" spans="1:7" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="37"/>
-      <c r="B46" s="37"/>
-      <c r="C46" s="37"/>
-      <c r="D46" s="37"/>
-      <c r="E46" s="37"/>
-      <c r="F46" s="37"/>
+      <c r="A46" s="29"/>
+      <c r="B46" s="29"/>
+      <c r="C46" s="29"/>
+      <c r="D46" s="29"/>
+      <c r="E46" s="29"/>
+      <c r="F46" s="29"/>
       <c r="G46" s="8"/>
     </row>
     <row r="47" spans="1:7" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A47" s="37"/>
-      <c r="B47" s="37"/>
-      <c r="C47" s="37"/>
-      <c r="D47" s="37"/>
-      <c r="E47" s="37"/>
-      <c r="F47" s="37"/>
+      <c r="A47" s="29"/>
+      <c r="B47" s="29"/>
+      <c r="C47" s="29"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="29"/>
+      <c r="F47" s="29"/>
       <c r="G47" s="8"/>
     </row>
     <row r="48" spans="1:7" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A48" s="37"/>
-      <c r="B48" s="37"/>
-      <c r="C48" s="37"/>
-      <c r="D48" s="37"/>
-      <c r="E48" s="37"/>
-      <c r="F48" s="37"/>
+      <c r="A48" s="29"/>
+      <c r="B48" s="29"/>
+      <c r="C48" s="29"/>
+      <c r="D48" s="29"/>
+      <c r="E48" s="29"/>
+      <c r="F48" s="29"/>
       <c r="G48" s="8"/>
     </row>
     <row r="49" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
@@ -1316,6 +1332,15 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="H8:M8"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
     <mergeCell ref="A46:F46"/>
     <mergeCell ref="A47:F47"/>
     <mergeCell ref="A48:F48"/>
@@ -1325,15 +1350,6 @@
     <mergeCell ref="A43:F43"/>
     <mergeCell ref="A44:F44"/>
     <mergeCell ref="A45:F45"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="A40:F40"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="H8:M8"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>